<commit_message>
10.245.10.37 M drive assessed
</commit_message>
<xml_diff>
--- a/Disk space reporting.xlsx
+++ b/Disk space reporting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TichaonaMasanga\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TichaonaMasanga\Documents\Ekwantu\SQL scripts\sql_script_backups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B56845-ABAC-4F24-8654-B3D1FA45FB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A977E-881D-46C8-B9CC-9035C729C4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9064F82D-B6FE-45BE-9862-B0A59B5F005C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>erver</t>
   </si>
@@ -113,7 +113,16 @@
     <t>Auto growth disabled. Risk of outage removed</t>
   </si>
   <si>
-    <t>Data pointed to drive with space, and there is and old db that needs to be removed. Its backed up on 10.160 this is pending Mr Jose's approval. Auto growth disabled. Risk of outage removed</t>
+    <t>10.245.10.37</t>
+  </si>
+  <si>
+    <t>M:\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Auto growth disabled. Risk of outage removed</t>
+  </si>
+  <si>
+    <t>Data pointed to drive with space, and there is and old db that needs to be removed. Its backed up on 10.160 this is pending Mr Jose's approval.</t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A9FF04-5E2E-4B02-94FE-50AFAEF1451B}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,7 +577,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -639,6 +648,17 @@
       </c>
       <c r="D8" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10.245.10.37 M drive assessed and comment about STBMZ_eBankitMonitoringHistory_Old added
</commit_message>
<xml_diff>
--- a/Disk space reporting.xlsx
+++ b/Disk space reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TichaonaMasanga\Documents\Ekwantu\SQL scripts\sql_script_backups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A977E-881D-46C8-B9CC-9035C729C4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3632C2AE-AF25-467E-89A1-24B675BD178E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9064F82D-B6FE-45BE-9862-B0A59B5F005C}"/>
   </bookViews>
@@ -122,7 +122,7 @@
     <t xml:space="preserve"> Auto growth disabled. Risk of outage removed</t>
   </si>
   <si>
-    <t>Data pointed to drive with space, and there is and old db that needs to be removed. Its backed up on 10.160 this is pending Mr Jose's approval.</t>
+    <t>Data pointed to drive with space, and there is and old db (STBMZ_eBankitMonitoringHistory_Old) that needs to be removed. Its backed up on 10.160 this is pending Mr Jose's approval.</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>